<commit_message>
Trabajo en el Lab
</commit_message>
<xml_diff>
--- a/Lancaster/Reporte_02_Q-Preliminar/QMatriz_Own.xlsx
+++ b/Lancaster/Reporte_02_Q-Preliminar/QMatriz_Own.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\Desktop\afchavez19\Lancaster\Reporte_02_Q-Preliminar\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="12435"/>
   </bookViews>
@@ -613,7 +618,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -621,12 +626,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AL53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:C50"/>
+      <selection pane="bottomLeft" activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,7 +757,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -803,7 +807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -853,7 +857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -900,7 +904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -947,7 +951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1079,7 +1083,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1167,7 +1171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1214,7 +1218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1261,7 +1265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1352,7 +1356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1402,7 +1406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1449,7 +1453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1496,7 +1500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1543,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1634,7 +1638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1684,7 +1688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1734,7 +1738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1781,7 +1785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1831,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1881,7 +1885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1931,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2022,7 +2026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2072,7 +2076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2201,7 +2205,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2248,7 +2252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2295,7 +2299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2342,7 +2346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2392,7 +2396,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2439,7 +2443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2486,7 +2490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2577,7 +2581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2668,7 +2672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2715,7 +2719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2765,7 +2769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2815,7 +2819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2865,7 +2869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2915,7 +2919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:38" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2962,7 +2966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3012,7 +3016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:38" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3134,16 +3138,7 @@
       <c r="AL53" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL51">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="2 - MI"/>
-      </filters>
-    </filterColumn>
-    <sortState ref="A2:AL51">
-      <sortCondition ref="A1:A51"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:AL51"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>